<commit_message>
Facing issue in updating project. Still working on modules.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginData.xlsx
+++ b/src/test/resources/testdata/LoginData.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankush\eclipse-workspace\GSIT_Automation_Testing\SeleniumFramework_Ankush\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CF3056-526C-4AAB-BCD8-8B14126CFE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -19,34 +28,46 @@
     <t>password</t>
   </si>
   <si>
-    <t>Admin@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin@123</t>
-  </si>
-  <si>
     <t>Admin@1234</t>
+  </si>
+  <si>
+    <t>admin_ankush@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@admin</t>
+  </si>
+  <si>
+    <t>admin_new@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,11 +75,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF888888"/>
@@ -72,35 +99,40 @@
       <bottom style="thin">
         <color rgb="FF888888"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -290,24 +322,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="24.0"/>
-    <col customWidth="1" min="2" max="2" width="19.13"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="19.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -315,23 +352,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1E6BF740-0DA0-4972-AC2D-673990306F76}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>